<commit_message>
Tried fixing the bug
</commit_message>
<xml_diff>
--- a/records.xlsx
+++ b/records.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK2"/>
+  <dimension ref="A1:AK3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -667,6 +667,53 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr"/>
+      <c r="AB3" t="inlineStr"/>
+      <c r="AC3" t="inlineStr"/>
+      <c r="AD3" t="inlineStr"/>
+      <c r="AE3" t="inlineStr"/>
+      <c r="AF3" t="inlineStr"/>
+      <c r="AG3" t="inlineStr"/>
+      <c r="AH3" t="inlineStr"/>
+      <c r="AI3" t="inlineStr"/>
+      <c r="AJ3" t="inlineStr">
+        <is>
+          <t>user1</t>
+        </is>
+      </c>
+      <c r="AK3" t="inlineStr">
+        <is>
+          <t>2025-01-31</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>